<commit_message>
uploaded fsr s4 test data from 15may24
</commit_message>
<xml_diff>
--- a/data/FSR_S4/calibration/FSR_S4 Calibration Data.xlsx
+++ b/data/FSR_S4/calibration/FSR_S4 Calibration Data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/patrickruiz/Desktop/FSR/data/FSR_S4/calibration/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://amro365-my.sharepoint.com/personal/pr19556_appliedmed_com/Documents/Desktop/FSR/data/FSR_S4/calibration/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{943968B9-7CAD-6F4A-8B61-C7855A75CDE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="880" windowWidth="36000" windowHeight="22500" xr2:uid="{A44B9C34-151F-4DB5-ABDC-540135FA09DD}"/>
+    <workbookView xWindow="1080" yWindow="2595" windowWidth="21600" windowHeight="11160" xr2:uid="{A44B9C34-151F-4DB5-ABDC-540135FA09DD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -153,9 +153,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -193,7 +193,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -299,7 +299,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -441,7 +441,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -452,23 +452,23 @@
   <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.83203125" style="2"/>
-    <col min="2" max="2" width="14.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.83203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="8.83203125" style="2"/>
+    <col min="1" max="1" width="8.85546875" style="2"/>
+    <col min="2" max="2" width="14.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="8.85546875" style="2"/>
     <col min="6" max="6" width="8" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.1640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="27.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="16384" width="8.83203125" style="2"/>
+    <col min="7" max="7" width="12.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="27.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="8.85546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -497,7 +497,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>9</v>
       </c>
@@ -524,7 +524,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
@@ -533,7 +533,7 @@
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
@@ -542,7 +542,7 @@
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
@@ -551,7 +551,7 @@
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B7" s="3"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
did more analysis on fsrs4 day2
</commit_message>
<xml_diff>
--- a/data/FSR_S4/calibration/FSR_S4 Calibration Data.xlsx
+++ b/data/FSR_S4/calibration/FSR_S4 Calibration Data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://amro365-my.sharepoint.com/personal/pr19556_appliedmed_com/Documents/Desktop/FSR/data/FSR_S4/calibration/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pr19556\OneDrive - Applied Medical\Desktop\FSR\data\FSR_S4\calibration\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{943968B9-7CAD-6F4A-8B61-C7855A75CDE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33F036B4-7983-43BA-BB27-7682F59CE287}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1080" yWindow="2595" windowWidth="21600" windowHeight="11160" xr2:uid="{A44B9C34-151F-4DB5-ABDC-540135FA09DD}"/>
+    <workbookView xWindow="3060" yWindow="2295" windowWidth="21600" windowHeight="11160" xr2:uid="{A44B9C34-151F-4DB5-ABDC-540135FA09DD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
   <si>
     <t>FSR</t>
   </si>
@@ -69,6 +69,12 @@
   </si>
   <si>
     <t>After Stability Testing from (4-9lb)</t>
+  </si>
+  <si>
+    <t>After 4.5lbf Load Overnight</t>
+  </si>
+  <si>
+    <t>After 2nd Day Testing</t>
   </si>
 </sst>
 </file>
@@ -452,7 +458,7 @@
   <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -464,7 +470,7 @@
     <col min="6" max="6" width="8" style="2" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12.140625" style="2" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="16.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="27.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="31.85546875" style="2" bestFit="1" customWidth="1"/>
     <col min="10" max="16384" width="8.85546875" style="2"/>
   </cols>
   <sheetData>
@@ -525,22 +531,58 @@
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
+      <c r="A3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="1">
+        <v>19001.27377</v>
+      </c>
+      <c r="C3" s="1">
+        <v>105.02494</v>
+      </c>
+      <c r="D3" s="1">
+        <v>-1.0072099999999999</v>
+      </c>
+      <c r="E3" s="1">
+        <v>3.0200000000000001E-3</v>
+      </c>
+      <c r="F3" s="1">
+        <v>0.99885000000000002</v>
+      </c>
+      <c r="G3" s="1">
+        <v>7361.0400900000004</v>
+      </c>
       <c r="H3" s="1"/>
+      <c r="I3" s="1" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
+      <c r="A4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="1">
+        <v>18185.953440000001</v>
+      </c>
+      <c r="C4" s="1">
+        <v>117.52136</v>
+      </c>
+      <c r="D4" s="1">
+        <v>-0.99470999999999998</v>
+      </c>
+      <c r="E4" s="1">
+        <v>3.5300000000000002E-3</v>
+      </c>
+      <c r="F4" s="1">
+        <v>1</v>
+      </c>
+      <c r="G4" s="1">
+        <v>9656.0690900000009</v>
+      </c>
       <c r="H4" s="1"/>
+      <c r="I4" s="1" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B5" s="1"/>

</xml_diff>

<commit_message>
created function to round sigfigs
</commit_message>
<xml_diff>
--- a/data/FSR_S4/calibration/FSR_S4 Calibration Data.xlsx
+++ b/data/FSR_S4/calibration/FSR_S4 Calibration Data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pr19556\OneDrive - Applied Medical\Desktop\FSR\data\FSR_S4\calibration\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/patrickruiz/Desktop/FSR/data/FSR_S4/calibration/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33F036B4-7983-43BA-BB27-7682F59CE287}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4200DCBC-888F-DF4C-8075-A9193F892908}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3060" yWindow="2295" windowWidth="21600" windowHeight="11160" xr2:uid="{A44B9C34-151F-4DB5-ABDC-540135FA09DD}"/>
+    <workbookView xWindow="0" yWindow="860" windowWidth="36000" windowHeight="22520" xr2:uid="{A44B9C34-151F-4DB5-ABDC-540135FA09DD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -124,7 +124,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -136,9 +136,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -159,9 +156,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -199,7 +196,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -305,7 +302,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -447,7 +444,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -458,23 +455,23 @@
   <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="8.85546875" style="2"/>
-    <col min="2" max="2" width="14.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="8.85546875" style="2"/>
+    <col min="1" max="1" width="8.83203125" style="2"/>
+    <col min="2" max="2" width="14.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="8.83203125" style="2"/>
     <col min="6" max="6" width="8" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="31.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="16384" width="8.85546875" style="2"/>
+    <col min="7" max="7" width="12.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="31.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="8.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -503,7 +500,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>9</v>
       </c>
@@ -526,11 +523,11 @@
         <v>4190.6651700000002</v>
       </c>
       <c r="H2" s="1"/>
-      <c r="I2" s="5" t="s">
+      <c r="I2" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>9</v>
       </c>
@@ -557,7 +554,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
@@ -584,7 +581,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
@@ -593,7 +590,7 @@
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B7" s="3"/>
     </row>
   </sheetData>

</xml_diff>